<commit_message>
update to remove OpenCV
</commit_message>
<xml_diff>
--- a/gantt-chart.xlsx
+++ b/gantt-chart.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acreg\Desktop\final year\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acreg\Desktop\final_year\Project\ImageSearchEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6034A97-8BDB-4E7F-BE7E-7433EC2AAB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA4F5D5-130B-4B89-834D-989DAEC2EE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
+    <sheet name="GanttChart updated" sheetId="10" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!#REF!</definedName>
@@ -99,8 +100,69 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Vertex42</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{45305954-241E-4336-B91C-6907FA7835F6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Work Breakdown Structure</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Level 1: 1, 2, 3, ...
+Level 2: 1.1, 1.2, 1.3, ...
+Level 3: 1.1.1, 1.1.2, 1.1.3, …
+ - The WBS uses a formula to control the numbering, but the formulas are different for different levels. Copy and Paste the cells in the WBS column from the examples at the bottom of the worksheet.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{8376EF54-A643-408E-9CDE-B1AD8FBDAAD4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Predecessor Tasks:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>You can use this column to enter the WBS of a predecessor for reference. The PRO version uses formulas to automatically calculate the Start Date based on the Predecessor.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="25">
   <si>
     <t>TASK</t>
   </si>
@@ -781,68 +843,64 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1027,6 +1085,65 @@
         <a:effectLst>
           <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
             <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8228" name="Text Box 36" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BAC91EA-878E-D9A5-327A-0872405B414C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2232660" y="464820"/>
+          <a:ext cx="2903220" cy="1242060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFE1" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="80"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="510000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="510000"/>
           </a:outerShdw>
         </a:effectLst>
         <a:extLst>
@@ -1333,325 +1450,339 @@
   </sheetPr>
   <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:B17"/>
+      <selection pane="bottomLeft" activeCell="U18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" style="2" customWidth="1"/>
-    <col min="7" max="28" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" customWidth="1"/>
+    <col min="7" max="28" width="4.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="18" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="20" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="20" t="s">
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="20" t="s">
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="20" t="s">
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="20" t="s">
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17"/>
-    </row>
-    <row r="3" spans="1:28" s="11" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+    </row>
+    <row r="3" spans="1:28" s="7" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="Q3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="R3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="S3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="T3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="U3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="V3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="W3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="X3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="Y3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="Z3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AA3" s="16" t="s">
+      <c r="AA3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AB3" s="16" t="s">
+      <c r="AB3" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-    </row>
-    <row r="5" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="13"/>
-      <c r="F5" s="26"/>
-    </row>
-    <row r="6" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="13"/>
-      <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="9"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="13"/>
-      <c r="H7" s="26"/>
-    </row>
-    <row r="8" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="9"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="8"/>
-      <c r="H8" s="26"/>
-    </row>
-    <row r="9" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="4"/>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="13"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-    </row>
-    <row r="10" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="13"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-    </row>
-    <row r="11" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="9"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+    </row>
+    <row r="11" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="13"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-    </row>
-    <row r="12" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="9"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+    </row>
+    <row r="12" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="13"/>
-      <c r="R12" s="26"/>
-    </row>
-    <row r="13" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="9"/>
+      <c r="R12" s="19"/>
+    </row>
+    <row r="13" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="13"/>
-      <c r="S13" s="26"/>
-    </row>
-    <row r="14" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="9"/>
+      <c r="S13" s="19"/>
+    </row>
+    <row r="14" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="8"/>
-      <c r="T14" s="26"/>
-    </row>
-    <row r="15" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="13"/>
-    </row>
-    <row r="16" spans="1:28" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="13"/>
-    </row>
-    <row r="17" spans="1:3" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="13"/>
-    </row>
-    <row r="18" spans="1:3" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="13"/>
-    </row>
-    <row r="19" spans="1:3" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="13"/>
-    </row>
-    <row r="20" spans="1:3" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:3" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="13"/>
-    </row>
-    <row r="22" spans="1:3" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="13"/>
-    </row>
-    <row r="23" spans="1:3" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="13"/>
-    </row>
-    <row r="24" spans="1:3" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="13"/>
-    </row>
-    <row r="25" spans="1:3" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="13"/>
-    </row>
-    <row r="26" spans="1:3" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" spans="1:3" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="8"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="4"/>
+      <c r="T14" s="19"/>
+    </row>
+    <row r="15" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" s="5" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" s="5" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="4"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="23">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
@@ -1660,21 +1791,6 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.25"/>
@@ -1686,4 +1802,353 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04833162-724A-4CED-85E4-1E1310BC37EB}">
+  <dimension ref="A1:AB27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" customWidth="1"/>
+    <col min="7" max="28" width="4.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+    </row>
+    <row r="3" spans="1:28" s="7" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB3" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="9"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="9"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="4"/>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="9"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+    </row>
+    <row r="11" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="9"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+    </row>
+    <row r="12" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="9"/>
+      <c r="R12" s="19"/>
+    </row>
+    <row r="13" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="9"/>
+      <c r="S13" s="19"/>
+    </row>
+    <row r="14" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="4"/>
+      <c r="T14" s="19"/>
+    </row>
+    <row r="15" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:28" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" s="5" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" s="5" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>